<commit_message>
update admin audit it
</commit_message>
<xml_diff>
--- a/BackEnd_RMA/uploads/SPI.xlsx
+++ b/BackEnd_RMA/uploads/SPI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\file rolan\File Kuliah\Manajement-Audit-PT-DI\BackEnd_RMA\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\file rolan\File Kuliah\KP\BackEnd_RMA\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB645A0-0CD2-4731-9EF7-6D6BB614BC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF29C987-43D5-49DC-A655-30DDC9FC312D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8C6427D0-B0C2-4D4B-AB94-AF9B666D475E}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,9 +512,6 @@
       <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2">
-        <v>32131</v>
-      </c>
       <c r="H2">
         <v>1</v>
       </c>
@@ -538,9 +535,6 @@
       <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="G3">
-        <v>23213</v>
-      </c>
       <c r="H3">
         <v>2</v>
       </c>
@@ -564,9 +558,6 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4">
-        <v>21312</v>
-      </c>
       <c r="H4">
         <v>3</v>
       </c>
@@ -590,9 +581,6 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5">
-        <v>21321</v>
-      </c>
       <c r="H5">
         <v>3</v>
       </c>
@@ -616,9 +604,6 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6">
-        <v>21312</v>
-      </c>
       <c r="H6">
         <v>4</v>
       </c>
@@ -641,9 +626,6 @@
       </c>
       <c r="F7" t="s">
         <v>17</v>
-      </c>
-      <c r="G7">
-        <v>21332</v>
       </c>
       <c r="H7">
         <v>4</v>

</xml_diff>